<commit_message>
update voc and hrms
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/Ehs_NoiDungDemucChiTietTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/Ehs_NoiDungDemucChiTietTemplate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Nhà Thầu</t>
   </si>
@@ -128,6 +128,18 @@
       </rPr>
       <t>2022-09-10</t>
     </r>
+  </si>
+  <si>
+    <t>Mã hiệu máy kiểm tra</t>
+  </si>
+  <si>
+    <t>Kết quả</t>
+  </si>
+  <si>
+    <t>Chi phí(Số tiền)</t>
+  </si>
+  <si>
+    <t>Tiến độ hoàn thành(%)</t>
   </si>
 </sst>
 </file>
@@ -176,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -199,11 +211,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -217,6 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,19 +524,19 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="16" width="31.7109375" customWidth="1"/>
+    <col min="2" max="18" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -529,31 +553,43 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="O1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="3" t="s">
@@ -565,26 +601,32 @@
       <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="5">
+      <c r="K2" s="3"/>
+      <c r="L2" s="5">
         <v>42377</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>2</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="O2" s="3">
+        <v>50</v>
+      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -596,7 +638,7 @@
           <x14:formula1>
             <xm:f>DMY!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2 M2</xm:sqref>
+          <xm:sqref>E2:F2 N2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>